<commit_message>
Additional updates to data dictionary
</commit_message>
<xml_diff>
--- a/Source Data/LCDataDictionary.xlsx
+++ b/Source Data/LCDataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/littlemac/Documents/S109/Final-Project/Source Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D941714-29D4-164E-A5BB-DAFCB697FDCC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B48F10-71C9-4442-9F4E-4F112B75D40C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24800" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2330,9 +2330,9 @@
   </sheetPr>
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D118" sqref="D118:D152"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update from last weekend
</commit_message>
<xml_diff>
--- a/Source Data/LCDataDictionary.xlsx
+++ b/Source Data/LCDataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/littlemac/Documents/S109/Final-Project/Source Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pareddy/pavio/Personal Documents/courses/cs109a/Final-Project/Source Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B48F10-71C9-4442-9F4E-4F112B75D40C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B659BFCF-175C-AA49-9AC8-98BCD6D0A726}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24800" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$E$154</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$F$154</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="408">
   <si>
     <t>id</t>
   </si>
@@ -1269,6 +1269,9 @@
   </si>
   <si>
     <t>sec_app_num_rev_accts</t>
+  </si>
+  <si>
+    <t>Kaggle</t>
   </si>
 </sst>
 </file>
@@ -2328,23 +2331,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L154"/>
+  <dimension ref="A1:M154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.1640625" customWidth="1"/>
-    <col min="3" max="3" width="158.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" customWidth="1"/>
+    <col min="4" max="5" width="11.33203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="16" t="s">
         <v>99</v>
       </c>
@@ -2354,11 +2357,14 @@
       <c r="D1" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -2371,11 +2377,12 @@
       <c r="D2" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2388,8 +2395,9 @@
       <c r="D3" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -2403,10 +2411,13 @@
         <v>385</v>
       </c>
       <c r="E4" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -2419,9 +2430,9 @@
       <c r="D5" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -2434,8 +2445,11 @@
       <c r="D6" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -2446,10 +2460,11 @@
         <v>265</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -2462,8 +2477,9 @@
       <c r="D8" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -2476,11 +2492,12 @@
       <c r="D9" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -2493,8 +2510,9 @@
       <c r="D10" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -2507,11 +2525,12 @@
       <c r="D11" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -2524,8 +2543,9 @@
       <c r="D12" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -2538,8 +2558,9 @@
       <c r="D13" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -2552,8 +2573,9 @@
       <c r="D14" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -2566,8 +2588,11 @@
       <c r="D15" s="24" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -2580,11 +2605,12 @@
       <c r="D16" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="13"/>
+      <c r="F16" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -2597,8 +2623,11 @@
       <c r="D17" s="5" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -2611,8 +2640,11 @@
       <c r="D18" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -2623,10 +2655,11 @@
         <v>256</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -2637,10 +2670,13 @@
         <v>249</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -2653,8 +2689,11 @@
       <c r="D21" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -2665,10 +2704,13 @@
         <v>167</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -2681,11 +2723,12 @@
       <c r="D23" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="5"/>
+      <c r="F23" s="25" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -2698,8 +2741,9 @@
       <c r="D24" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2712,8 +2756,9 @@
       <c r="D25" s="5" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -2726,8 +2771,9 @@
       <c r="D26" s="5" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -2738,10 +2784,13 @@
         <v>60</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -2754,8 +2803,11 @@
       <c r="D28" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -2768,8 +2820,11 @@
       <c r="D29" s="24" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -2782,11 +2837,12 @@
       <c r="D30" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="6"/>
+      <c r="F30" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -2799,8 +2855,9 @@
       <c r="D31" s="5" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -2813,8 +2870,11 @@
       <c r="D32" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E32" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2827,8 +2887,9 @@
       <c r="D33" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -2841,8 +2902,11 @@
       <c r="D34" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E34" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -2856,10 +2920,13 @@
         <v>384</v>
       </c>
       <c r="E35" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="F35" s="25" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -2872,8 +2939,11 @@
       <c r="D36" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E36" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -2884,12 +2954,13 @@
         <v>248</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="J37" s="10"/>
-      <c r="K37" s="11"/>
-    </row>
-    <row r="38" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -2902,8 +2973,9 @@
       <c r="D38" s="5" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -2916,11 +2988,12 @@
       <c r="D39" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E39" s="25" t="s">
+      <c r="E39" s="5"/>
+      <c r="F39" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -2933,11 +3006,12 @@
       <c r="D40" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E40" s="25" t="s">
+      <c r="E40" s="5"/>
+      <c r="F40" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -2950,11 +3024,12 @@
       <c r="D41" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E41" s="25" t="s">
+      <c r="E41" s="5"/>
+      <c r="F41" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -2967,11 +3042,12 @@
       <c r="D42" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E42" s="25" t="s">
+      <c r="E42" s="5"/>
+      <c r="F42" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -2984,9 +3060,12 @@
       <c r="D43" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E43" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -2999,11 +3078,14 @@
       <c r="D44" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E44" s="25" t="s">
+      <c r="E44" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="F44" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -3016,11 +3098,11 @@
       <c r="D45" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E45" s="25" t="s">
+      <c r="F45" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -3033,12 +3115,13 @@
       <c r="D46" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E46" s="25"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="11"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="25"/>
+      <c r="K46" s="10"/>
       <c r="L46" s="11"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" s="11"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -3051,12 +3134,13 @@
       <c r="D47" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="11"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="4"/>
+      <c r="K47" s="10"/>
       <c r="L47" s="11"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" s="11"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -3069,12 +3153,13 @@
       <c r="D48" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E48" s="4"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="11"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="4"/>
+      <c r="K48" s="12"/>
       <c r="L48" s="11"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="M48" s="11"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -3087,9 +3172,10 @@
       <c r="D49" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E49" s="5"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -3102,9 +3188,10 @@
       <c r="D50" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E50" s="5"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -3117,9 +3204,10 @@
       <c r="D51" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E51" s="5"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -3132,9 +3220,12 @@
       <c r="D52" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E52" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -3147,9 +3238,12 @@
       <c r="D53" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E53" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -3162,9 +3256,12 @@
       <c r="D54" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E54" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -3177,9 +3274,10 @@
       <c r="D55" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="5"/>
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -3192,9 +3290,10 @@
       <c r="D56" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E56" s="4"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E56" s="5"/>
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -3207,9 +3306,10 @@
       <c r="D57" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E57" s="4"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="5"/>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -3222,9 +3322,10 @@
       <c r="D58" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E58" s="4"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E58" s="5"/>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -3237,9 +3338,10 @@
       <c r="D59" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E59" s="4"/>
-    </row>
-    <row r="60" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E59" s="5"/>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -3252,9 +3354,10 @@
       <c r="D60" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E60" s="4"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E60" s="5"/>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -3267,9 +3370,10 @@
       <c r="D61" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E61" s="4"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E61" s="5"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -3282,11 +3386,11 @@
       <c r="D62" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E62" s="25" t="s">
+      <c r="F62" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -3299,11 +3403,11 @@
       <c r="D63" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E63" s="25" t="s">
+      <c r="F63" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -3316,8 +3420,9 @@
       <c r="D64" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -3330,8 +3435,9 @@
       <c r="D65" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>64</v>
       </c>
@@ -3344,8 +3450,9 @@
       <c r="D66" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>65</v>
       </c>
@@ -3358,8 +3465,9 @@
       <c r="D67" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E67" s="5"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>66</v>
       </c>
@@ -3372,8 +3480,9 @@
       <c r="D68" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>67</v>
       </c>
@@ -3386,8 +3495,9 @@
       <c r="D69" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E69" s="5"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>68</v>
       </c>
@@ -3400,8 +3510,9 @@
       <c r="D70" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>69</v>
       </c>
@@ -3414,11 +3525,11 @@
       <c r="D71" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E71" s="25" t="s">
+      <c r="F71" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>70</v>
       </c>
@@ -3431,11 +3542,11 @@
       <c r="D72" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E72" s="25" t="s">
+      <c r="F72" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>71</v>
       </c>
@@ -3448,9 +3559,10 @@
       <c r="D73" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="G73" s="6"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E73" s="5"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>72</v>
       </c>
@@ -3463,8 +3575,9 @@
       <c r="D74" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>73</v>
       </c>
@@ -3477,8 +3590,11 @@
       <c r="D75" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E75" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>74</v>
       </c>
@@ -3491,8 +3607,9 @@
       <c r="D76" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>75</v>
       </c>
@@ -3505,8 +3622,9 @@
       <c r="D77" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E77" s="5"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>76</v>
       </c>
@@ -3519,8 +3637,9 @@
       <c r="D78" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>77</v>
       </c>
@@ -3533,11 +3652,11 @@
       <c r="D79" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E79" s="25" t="s">
+      <c r="F79" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>78</v>
       </c>
@@ -3550,8 +3669,9 @@
       <c r="D80" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>79</v>
       </c>
@@ -3564,8 +3684,9 @@
       <c r="D81" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>80</v>
       </c>
@@ -3578,8 +3699,9 @@
       <c r="D82" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" s="5"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>81</v>
       </c>
@@ -3592,8 +3714,9 @@
       <c r="D83" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" s="5"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>82</v>
       </c>
@@ -3606,8 +3729,9 @@
       <c r="D84" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" s="5"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>83</v>
       </c>
@@ -3620,8 +3744,9 @@
       <c r="D85" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="E85" s="5"/>
+    </row>
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>84</v>
       </c>
@@ -3634,8 +3759,9 @@
       <c r="D86" s="5" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" s="5"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>85</v>
       </c>
@@ -3648,8 +3774,11 @@
       <c r="D87" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>86</v>
       </c>
@@ -3662,8 +3791,9 @@
       <c r="D88" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" s="5"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>87</v>
       </c>
@@ -3674,10 +3804,13 @@
         <v>237</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+      <c r="E89" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>88</v>
       </c>
@@ -3690,8 +3823,11 @@
       <c r="D90" s="6" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>89</v>
       </c>
@@ -3705,7 +3841,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>90</v>
       </c>
@@ -3718,8 +3854,11 @@
       <c r="D92" s="6" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>91</v>
       </c>
@@ -3732,8 +3871,11 @@
       <c r="D93" s="6" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>92</v>
       </c>
@@ -3746,8 +3888,11 @@
       <c r="D94" s="6" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>93</v>
       </c>
@@ -3761,7 +3906,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>94</v>
       </c>
@@ -3774,8 +3919,11 @@
       <c r="D96" s="6" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E96" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>95</v>
       </c>
@@ -3788,8 +3936,11 @@
       <c r="D97" s="6" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E97" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>96</v>
       </c>
@@ -3803,7 +3954,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>97</v>
       </c>
@@ -3816,11 +3967,11 @@
       <c r="D99" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E99" s="25" t="s">
+      <c r="F99" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>98</v>
       </c>
@@ -3834,7 +3985,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>99</v>
       </c>
@@ -3847,11 +3998,14 @@
       <c r="D101" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E101" s="25" t="s">
+      <c r="E101" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="F101" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>100</v>
       </c>
@@ -3865,7 +4019,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>101</v>
       </c>
@@ -3878,11 +4032,11 @@
       <c r="D103" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E103" s="25" t="s">
+      <c r="F103" s="25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>102</v>
       </c>
@@ -3896,7 +4050,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>103</v>
       </c>
@@ -3910,7 +4064,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>104</v>
       </c>
@@ -3924,7 +4078,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>105</v>
       </c>
@@ -3937,11 +4091,11 @@
       <c r="D107" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="E107" s="10" t="s">
+      <c r="F107" s="10" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>106</v>
       </c>
@@ -3954,11 +4108,11 @@
       <c r="D108" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E108" s="10" t="s">
+      <c r="F108" s="10" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>107</v>
       </c>
@@ -3971,11 +4125,11 @@
       <c r="D109" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E109" s="10" t="s">
+      <c r="F109" s="10" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>108</v>
       </c>
@@ -3988,11 +4142,11 @@
       <c r="D110" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E110" s="10" t="s">
+      <c r="F110" s="10" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>109</v>
       </c>
@@ -4005,11 +4159,11 @@
       <c r="D111" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E111" s="10" t="s">
+      <c r="F111" s="10" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>110</v>
       </c>
@@ -4022,9 +4176,9 @@
       <c r="D112" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="E112" s="10"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112" s="10"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>111</v>
       </c>
@@ -4037,9 +4191,12 @@
       <c r="D113" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E113" s="10"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E113" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="F113" s="10"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>112</v>
       </c>
@@ -4052,8 +4209,11 @@
       <c r="D114" s="6" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E114" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>113</v>
       </c>
@@ -4066,11 +4226,11 @@
       <c r="D115" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E115" s="10" t="s">
+      <c r="F115" s="10" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>114</v>
       </c>
@@ -4083,8 +4243,11 @@
       <c r="D116" s="6" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E116" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>115</v>
       </c>
@@ -4098,7 +4261,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>116</v>
       </c>
@@ -4111,9 +4274,9 @@
       <c r="D118" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E118" s="10"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118" s="10"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>117</v>
       </c>
@@ -4126,9 +4289,9 @@
       <c r="D119" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E119" s="10"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119" s="10"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>118</v>
       </c>
@@ -4142,7 +4305,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>119</v>
       </c>
@@ -4156,7 +4319,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>120</v>
       </c>
@@ -4170,7 +4333,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>121</v>
       </c>
@@ -4184,7 +4347,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>122</v>
       </c>
@@ -4197,9 +4360,9 @@
       <c r="D124" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E124" s="25"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F124" s="25"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>123</v>
       </c>
@@ -4212,9 +4375,9 @@
       <c r="D125" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="E125" s="25"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125" s="25"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>124</v>
       </c>
@@ -4228,7 +4391,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>125</v>
       </c>
@@ -4242,7 +4405,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>126</v>
       </c>
@@ -4606,7 +4769,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E154" xr:uid="{FF0C4084-7749-4411-8AD0-D248E5AF6185}"/>
+  <autoFilter ref="A1:F154" xr:uid="{FF0C4084-7749-4411-8AD0-D248E5AF6185}"/>
   <sortState ref="B2:C101">
     <sortCondition ref="B2:B101"/>
   </sortState>

</xml_diff>

<commit_message>
Added Neural net and random forest.
Added blocks ffor more advanced code with little success.
</commit_message>
<xml_diff>
--- a/Source Data/LCDataDictionary.xlsx
+++ b/Source Data/LCDataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpers\Documents\Developer\S109\Final-Project\Source Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA566BEF-1E3B-4453-B12A-D4A74BDBD14B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3208B57-9851-4465-918D-88EB402CFF95}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="75" yWindow="465" windowWidth="33525" windowHeight="20535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2341,7 +2341,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
+      <selection pane="bottomLeft" activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2392,7 +2392,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -2687,21 +2687,20 @@
     </row>
     <row r="20" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>384</v>
-      </c>
-      <c r="F20" s="25"/>
+        <v>118</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20"/>
     </row>
     <row r="21" spans="1:7" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -3779,7 +3778,7 @@
         <v>89</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
@@ -3795,7 +3794,7 @@
         <v>90</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
@@ -4175,7 +4174,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>105</v>
       </c>
@@ -4192,7 +4191,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>106</v>
       </c>
@@ -4393,17 +4392,22 @@
     </row>
     <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
-        <v>118</v>
-      </c>
-      <c r="B120" s="18" t="s">
-        <v>398</v>
-      </c>
-      <c r="C120" s="18" t="s">
-        <v>317</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>385</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="E120" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="F120" s="25"/>
+      <c r="G120" s="4"/>
     </row>
     <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
@@ -4872,10 +4876,12 @@
   <autoFilter ref="A1:G154" xr:uid="{FF0C4084-7749-4411-8AD0-D248E5AF6185}">
     <filterColumn colId="1">
       <filters>
-        <filter val="total_pymnt"/>
-        <filter val="total_pymnt_inv"/>
+        <filter val="acc_open_past_24mths"/>
       </filters>
     </filterColumn>
+    <sortState ref="A20:G120">
+      <sortCondition descending="1" ref="B1:B154"/>
+    </sortState>
   </autoFilter>
   <sortState ref="B2:C101">
     <sortCondition ref="B2:B101"/>

</xml_diff>

<commit_message>
Full data with interaction variables.
Note: (I commited while code was running. I will re-commit again in the morning.)
</commit_message>
<xml_diff>
--- a/Source Data/LCDataDictionary.xlsx
+++ b/Source Data/LCDataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpers\Documents\Developer\S109\Final-Project\Source Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B2B40D-98A6-49CB-9BE2-5C9064C54121}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFA0745-4CBE-472F-B70C-FC82A2BB53F1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="75" yWindow="465" windowWidth="33525" windowHeight="20535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2334,14 +2334,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D155" sqref="D155"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,7 +2373,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2408,7 +2408,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -2462,7 +2462,7 @@
       </c>
       <c r="F6" s="25"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -2478,7 +2478,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -2494,7 +2494,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -2529,7 +2529,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -2564,7 +2564,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -2580,7 +2580,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -2596,7 +2596,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -2614,7 +2614,7 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="F17" s="25"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="F18" s="25"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -2685,7 +2685,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>118</v>
       </c>
@@ -2702,7 +2702,7 @@
       <c r="F20" s="6"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="F21" s="25"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="F22" s="25"/>
     </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2789,7 +2789,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -2823,7 +2823,7 @@
       </c>
       <c r="F27" s="25"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="F28" s="25"/>
     </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="4" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -2912,7 +2912,7 @@
       </c>
       <c r="F32" s="25"/>
     </row>
-    <row r="33" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2928,7 +2928,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="F34" s="25"/>
     </row>
-    <row r="35" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="F36" s="25"/>
     </row>
-    <row r="37" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -3003,7 +3003,7 @@
       <c r="L37" s="10"/>
       <c r="M37" s="11"/>
     </row>
-    <row r="38" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -3019,7 +3019,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="F43" s="25"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -3172,7 +3172,7 @@
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -3192,7 +3192,7 @@
       <c r="M47" s="11"/>
       <c r="N47" s="11"/>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -3212,7 +3212,7 @@
       <c r="M48" s="11"/>
       <c r="N48" s="11"/>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -3229,7 +3229,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -3246,7 +3246,7 @@
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="4"/>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -3282,7 +3282,7 @@
       <c r="F52" s="25"/>
       <c r="G52" s="4"/>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -3301,7 +3301,7 @@
       <c r="F53" s="25"/>
       <c r="G53" s="4"/>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -3320,7 +3320,7 @@
       <c r="F54" s="25"/>
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -3337,7 +3337,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -3354,7 +3354,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -3371,7 +3371,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="4"/>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -3388,7 +3388,7 @@
       <c r="F58" s="5"/>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -3405,7 +3405,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="4"/>
     </row>
-    <row r="60" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -3422,7 +3422,7 @@
       <c r="F60" s="5"/>
       <c r="G60" s="4"/>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -3439,7 +3439,7 @@
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -3489,7 +3489,7 @@
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -3505,7 +3505,7 @@
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>64</v>
       </c>
@@ -3521,7 +3521,7 @@
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>65</v>
       </c>
@@ -3537,7 +3537,7 @@
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>66</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>67</v>
       </c>
@@ -3585,7 +3585,7 @@
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>69</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>70</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>71</v>
       </c>
@@ -3636,7 +3636,7 @@
       <c r="F73" s="5"/>
       <c r="I73" s="6"/>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>72</v>
       </c>
@@ -3652,7 +3652,7 @@
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>73</v>
       </c>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="F75" s="25"/>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>74</v>
       </c>
@@ -3686,7 +3686,7 @@
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>75</v>
       </c>
@@ -3702,7 +3702,7 @@
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>76</v>
       </c>
@@ -3718,7 +3718,7 @@
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>77</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>78</v>
       </c>
@@ -3751,7 +3751,7 @@
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>79</v>
       </c>
@@ -3767,7 +3767,7 @@
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>80</v>
       </c>
@@ -3783,7 +3783,7 @@
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>81</v>
       </c>
@@ -3799,7 +3799,7 @@
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>82</v>
       </c>
@@ -3815,7 +3815,7 @@
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>83</v>
       </c>
@@ -3831,7 +3831,7 @@
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
     </row>
-    <row r="86" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>84</v>
       </c>
@@ -3847,7 +3847,7 @@
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>85</v>
       </c>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="F87" s="25"/>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>86</v>
       </c>
@@ -3881,7 +3881,7 @@
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>87</v>
       </c>
@@ -3899,7 +3899,7 @@
       </c>
       <c r="F89" s="25"/>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>88</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="F90" s="10"/>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>89</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>90</v>
       </c>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="F92" s="10"/>
     </row>
-    <row r="93" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>91</v>
       </c>
@@ -3967,7 +3967,7 @@
       </c>
       <c r="F93" s="10"/>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>92</v>
       </c>
@@ -3985,7 +3985,7 @@
       </c>
       <c r="F94" s="10"/>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>93</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>94</v>
       </c>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="F96" s="10"/>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>95</v>
       </c>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="F97" s="10"/>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>96</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>97</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>98</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>99</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>100</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>101</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>102</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>103</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>104</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>105</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>106</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>107</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>108</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>109</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>110</v>
       </c>
@@ -4274,7 +4274,7 @@
       </c>
       <c r="G112" s="10"/>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>111</v>
       </c>
@@ -4293,7 +4293,7 @@
       <c r="F113" s="10"/>
       <c r="G113" s="10"/>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>112</v>
       </c>
@@ -4311,7 +4311,7 @@
       </c>
       <c r="F114" s="10"/>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>113</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>114</v>
       </c>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="F116" s="10"/>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>115</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>116</v>
       </c>
@@ -4375,7 +4375,7 @@
       </c>
       <c r="G118" s="10"/>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>117</v>
       </c>
@@ -4390,7 +4390,7 @@
       </c>
       <c r="G119" s="10"/>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>18</v>
       </c>
@@ -4409,7 +4409,7 @@
       <c r="F120" s="25"/>
       <c r="G120" s="4"/>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>119</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>120</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>121</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>122</v>
       </c>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="G124" s="25"/>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>123</v>
       </c>
@@ -4481,7 +4481,7 @@
       </c>
       <c r="G125" s="25"/>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>124</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>125</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>126</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>127</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>128</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>129</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>130</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>131</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>132</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>133</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>134</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>135</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>136</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>137</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>138</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>139</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>140</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>141</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>142</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>143</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>144</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>145</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>146</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>147</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>148</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>149</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>150</v>
       </c>
@@ -4859,12 +4859,12 @@
         <v>385</v>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>152</v>
       </c>
@@ -4874,11 +4874,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G154" xr:uid="{FF0C4084-7749-4411-8AD0-D248E5AF6185}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="num_sats"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A20:G120">
       <sortCondition descending="1" ref="B1:B154"/>
     </sortState>

</xml_diff>